<commit_message>
export excel dssv no mon
</commit_message>
<xml_diff>
--- a/04.Source/CapstoneMVC/src/main/resources/template/DSSV-học -lại.xlsx
+++ b/04.Source/CapstoneMVC/src/main/resources/template/DSSV-học -lại.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +55,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,7 +342,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="16384" width="9.23046875" style="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sửa lại template xuất DSSV Fail
</commit_message>
<xml_diff>
--- a/04.Source/CapstoneMVC/src/main/resources/template/DSSV-học -lại.xlsx
+++ b/04.Source/CapstoneMVC/src/main/resources/template/DSSV-học -lại.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,8 +62,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -73,6 +101,79 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="New Logo - Update01"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1847850" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,13 +441,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Xuất file dssv học lại, và lớp dự kiến học lại
</commit_message>
<xml_diff>
--- a/04.Source/CapstoneMVC/src/main/resources/template/DSSV-học -lại.xlsx
+++ b/04.Source/CapstoneMVC/src/main/resources/template/DSSV-học -lại.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12643"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DS môn Failed từng SV" sheetId="1" r:id="rId1"/>
+    <sheet name="Kế hoạch học lại" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,12 +19,71 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Danh sách các môn chưa đạt của từng sinh viên</t>
+  </si>
+  <si>
+    <t>MSSV</t>
+  </si>
+  <si>
+    <t>HỌ VÀ TÊN</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>CÁC MÔN CHƯA ĐẠT</t>
+  </si>
+  <si>
+    <t>MÃ MÔN</t>
+  </si>
+  <si>
+    <t>BỘ MÔN</t>
+  </si>
+  <si>
+    <t>SỐ LƯỢNG SV RỚT MÔN</t>
+  </si>
+  <si>
+    <t>SỐ LỚP DỰ KIẾN</t>
+  </si>
+  <si>
+    <t>Kế hoạch dự kiến</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -43,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -51,13 +111,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,13 +241,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1415204</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>212271</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -140,8 +271,81 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1847850" cy="762000"/>
+          <a:off x="0" y="1"/>
+          <a:ext cx="2487447" cy="947056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>968829</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="New Logo - Update01"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="0"/>
+          <a:ext cx="1986642" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -439,17 +643,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.3046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="15.15234375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.69140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.69140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="78.15234375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.3046875" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="19.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="19.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="19.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="19.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="14.3828125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.4609375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.84375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.4609375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.23046875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:C4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>